<commit_message>
Final del sprint 1
</commit_message>
<xml_diff>
--- a/Sprint 1/TPO Testing de aplicaciones (entrega 1 excel).xlsx
+++ b/Sprint 1/TPO Testing de aplicaciones (entrega 1 excel).xlsx
@@ -13,14 +13,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mgTskOPlFiezb+0jsK1kjgPN6OhyQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7miJ7ZTqKYfzPmZn025E+eAUV2Zc7g=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="211">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1130,7 +1130,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1270,6 +1270,12 @@
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
@@ -1321,9 +1327,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -2835,35 +2838,18 @@
       </c>
       <c r="C103" s="5"/>
       <c r="D103" s="50" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="E103" s="5"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="49">
-        <v>4.0</v>
-      </c>
-      <c r="B104" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="C104" s="5"/>
-      <c r="D104" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="E104" s="5"/>
+      <c r="A104" s="53"/>
+      <c r="B104" s="54"/>
+      <c r="D104" s="54"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
-      <c r="A105" s="49">
-        <v>5.0</v>
-      </c>
-      <c r="B105" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="C105" s="5"/>
-      <c r="D105" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="E105" s="5"/>
+      <c r="A105" s="53"/>
+      <c r="B105" s="54"/>
     </row>
     <row r="106" ht="14.25" customHeight="1"/>
     <row r="107" ht="14.25" customHeight="1">
@@ -4052,7 +4038,7 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="95">
+  <mergeCells count="94">
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="B35:C35"/>
@@ -4085,7 +4071,6 @@
     <mergeCell ref="D103:E103"/>
     <mergeCell ref="B104:C104"/>
     <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D105:E105"/>
     <mergeCell ref="D107:E107"/>
     <mergeCell ref="D108:E108"/>
     <mergeCell ref="B141:C141"/>
@@ -4173,39 +4158,39 @@
       <c r="B1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="56" t="s">
         <v>94</v>
       </c>
       <c r="E1" s="5"/>
     </row>
     <row r="2">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="60" t="s">
         <v>96</v>
       </c>
       <c r="E2" s="8"/>
     </row>
     <row r="3">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="62" t="s">
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="63" t="s">
+      <c r="E3" s="65" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="13"/>
@@ -4246,10 +4231,10 @@
       <c r="N5" s="13"/>
     </row>
     <row r="7">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="67" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="20" t="s">
@@ -4260,10 +4245,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="66">
+      <c r="A8" s="68">
         <v>1.0</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="69" t="s">
         <v>97</v>
       </c>
       <c r="D8" s="26">
@@ -4274,10 +4259,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="68">
+      <c r="A9" s="70">
         <v>2.0</v>
       </c>
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="71" t="s">
         <v>99</v>
       </c>
       <c r="D9" s="22">
@@ -4288,7 +4273,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="C10" s="70"/>
+      <c r="C10" s="72"/>
     </row>
     <row r="11">
       <c r="F11" s="13"/>
@@ -4514,9 +4499,9 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="71"/>
-      <c r="B21" s="71"/>
-      <c r="D21" s="71"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="53"/>
+      <c r="D21" s="53"/>
       <c r="G21" s="31"/>
       <c r="H21" s="32"/>
       <c r="I21" s="31"/>
@@ -4533,10 +4518,10 @@
       <c r="B22" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C22" s="53" t="s">
+      <c r="C22" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="72" t="s">
+      <c r="D22" s="73" t="s">
         <v>109</v>
       </c>
       <c r="E22" s="5"/>
@@ -4550,16 +4535,16 @@
       <c r="N22" s="32"/>
     </row>
     <row r="23">
-      <c r="A23" s="55" t="s">
+      <c r="A23" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="57" t="s">
+      <c r="C23" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="58" t="s">
+      <c r="D23" s="60" t="s">
         <v>96</v>
       </c>
       <c r="E23" s="8"/>
@@ -4573,15 +4558,15 @@
       <c r="N23" s="32"/>
     </row>
     <row r="24">
-      <c r="A24" s="59" t="s">
+      <c r="A24" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="60"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="62" t="s">
+      <c r="B24" s="62"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="73">
+      <c r="E24" s="74">
         <v>44563.0</v>
       </c>
     </row>
@@ -4635,17 +4620,17 @@
       <c r="N27" s="5"/>
     </row>
     <row r="28">
-      <c r="A28" s="64" t="s">
+      <c r="A28" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="65" t="s">
+      <c r="B28" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="74"/>
-      <c r="D28" s="75" t="s">
+      <c r="C28" s="75"/>
+      <c r="D28" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="76" t="s">
+      <c r="E28" s="77" t="s">
         <v>18</v>
       </c>
       <c r="G28" s="38"/>
@@ -4658,17 +4643,17 @@
       <c r="N28" s="5"/>
     </row>
     <row r="29">
-      <c r="A29" s="66">
+      <c r="A29" s="68">
         <v>1.0</v>
       </c>
-      <c r="B29" s="67" t="s">
+      <c r="B29" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="74"/>
-      <c r="D29" s="77">
+      <c r="C29" s="75"/>
+      <c r="D29" s="78">
         <v>1.0</v>
       </c>
-      <c r="E29" s="67" t="s">
+      <c r="E29" s="69" t="s">
         <v>111</v>
       </c>
       <c r="G29" s="38"/>
@@ -4681,17 +4666,17 @@
       <c r="N29" s="5"/>
     </row>
     <row r="30">
-      <c r="A30" s="68">
+      <c r="A30" s="70">
         <v>2.0</v>
       </c>
-      <c r="B30" s="69" t="s">
+      <c r="B30" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="74"/>
-      <c r="D30" s="77">
+      <c r="C30" s="75"/>
+      <c r="D30" s="78">
         <v>2.0</v>
       </c>
-      <c r="E30" s="78" t="s">
+      <c r="E30" s="79" t="s">
         <v>100</v>
       </c>
       <c r="G30" s="38"/>
@@ -4704,34 +4689,34 @@
       <c r="N30" s="5"/>
     </row>
     <row r="31">
-      <c r="A31" s="79"/>
-      <c r="B31" s="79"/>
-      <c r="C31" s="79"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
+      <c r="A31" s="80"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="80"/>
     </row>
     <row r="32">
-      <c r="A32" s="79"/>
-      <c r="B32" s="79"/>
-      <c r="C32" s="79"/>
-      <c r="D32" s="79"/>
-      <c r="E32" s="79"/>
+      <c r="A32" s="80"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
     </row>
     <row r="33">
-      <c r="A33" s="80"/>
-      <c r="B33" s="80"/>
-      <c r="C33" s="80"/>
-      <c r="D33" s="80"/>
-      <c r="E33" s="80"/>
+      <c r="A33" s="81"/>
+      <c r="B33" s="81"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="81"/>
     </row>
     <row r="34">
-      <c r="A34" s="81" t="s">
+      <c r="A34" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="82" t="s">
+      <c r="B34" s="83" t="s">
         <v>112</v>
       </c>
-      <c r="E34" s="83"/>
+      <c r="E34" s="84"/>
     </row>
     <row r="35">
       <c r="A35" s="39"/>
@@ -4742,44 +4727,44 @@
       <c r="F35" s="13"/>
     </row>
     <row r="36">
-      <c r="A36" s="84" t="s">
+      <c r="A36" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="80" t="s">
+      <c r="B36" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="85"/>
-      <c r="D36" s="86" t="s">
+      <c r="C36" s="86"/>
+      <c r="D36" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="87" t="s">
+      <c r="E36" s="88" t="s">
         <v>51</v>
       </c>
       <c r="F36" s="14"/>
     </row>
     <row r="37">
-      <c r="A37" s="80"/>
-      <c r="B37" s="80"/>
-      <c r="C37" s="80"/>
-      <c r="D37" s="80"/>
-      <c r="E37" s="80"/>
+      <c r="A37" s="81"/>
+      <c r="B37" s="81"/>
+      <c r="C37" s="81"/>
+      <c r="D37" s="81"/>
+      <c r="E37" s="81"/>
       <c r="F37" s="14"/>
     </row>
     <row r="38">
-      <c r="A38" s="88" t="s">
+      <c r="A38" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="89" t="s">
+      <c r="B38" s="90" t="s">
         <v>53</v>
       </c>
       <c r="C38" s="8"/>
-      <c r="D38" s="90" t="s">
+      <c r="D38" s="91" t="s">
         <v>54</v>
       </c>
       <c r="E38" s="8"/>
     </row>
     <row r="39">
-      <c r="A39" s="91">
+      <c r="A39" s="92">
         <v>1.0</v>
       </c>
       <c r="B39" s="50" t="s">
@@ -4790,10 +4775,10 @@
         <v>56</v>
       </c>
       <c r="E39" s="5"/>
-      <c r="F39" s="79"/>
+      <c r="F39" s="80"/>
     </row>
     <row r="40">
-      <c r="A40" s="91">
+      <c r="A40" s="92">
         <v>2.0</v>
       </c>
       <c r="B40" s="50" t="s">
@@ -4804,10 +4789,10 @@
         <v>114</v>
       </c>
       <c r="E40" s="5"/>
-      <c r="F40" s="79"/>
+      <c r="F40" s="80"/>
     </row>
     <row r="41">
-      <c r="A41" s="91">
+      <c r="A41" s="92">
         <v>3.0</v>
       </c>
       <c r="B41" s="50" t="s">
@@ -4818,10 +4803,10 @@
         <v>115</v>
       </c>
       <c r="E41" s="5"/>
-      <c r="F41" s="79"/>
+      <c r="F41" s="80"/>
     </row>
     <row r="42">
-      <c r="F42" s="79"/>
+      <c r="F42" s="80"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
@@ -4830,47 +4815,47 @@
       <c r="B43" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C43" s="53" t="s">
+      <c r="C43" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="72" t="s">
+      <c r="D43" s="73" t="s">
         <v>117</v>
       </c>
       <c r="E43" s="5"/>
-      <c r="F43" s="79"/>
+      <c r="F43" s="80"/>
     </row>
     <row r="44">
-      <c r="A44" s="55" t="s">
+      <c r="A44" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="57" t="s">
+      <c r="C44" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="92" t="s">
+      <c r="D44" s="93" t="s">
         <v>96</v>
       </c>
-      <c r="E44" s="80"/>
-      <c r="F44" s="79"/>
+      <c r="E44" s="81"/>
+      <c r="F44" s="80"/>
     </row>
     <row r="45">
-      <c r="A45" s="59" t="s">
+      <c r="A45" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="B45" s="60"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="62" t="s">
+      <c r="B45" s="62"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="E45" s="73">
+      <c r="E45" s="74">
         <v>44563.0</v>
       </c>
-      <c r="F45" s="79"/>
+      <c r="F45" s="80"/>
     </row>
     <row r="46">
-      <c r="F46" s="79"/>
+      <c r="F46" s="80"/>
     </row>
     <row r="47">
       <c r="A47" s="15" t="s">
@@ -4882,92 +4867,92 @@
       <c r="C47" s="14"/>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
-      <c r="F47" s="79"/>
+      <c r="F47" s="80"/>
     </row>
     <row r="48">
-      <c r="F48" s="79"/>
+      <c r="F48" s="80"/>
     </row>
     <row r="49">
-      <c r="A49" s="64" t="s">
+      <c r="A49" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="B49" s="93" t="s">
+      <c r="B49" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="C49" s="74"/>
-      <c r="D49" s="75" t="s">
+      <c r="C49" s="75"/>
+      <c r="D49" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="E49" s="76" t="s">
+      <c r="E49" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="F49" s="79"/>
+      <c r="F49" s="80"/>
     </row>
     <row r="50">
-      <c r="A50" s="94">
+      <c r="A50" s="95">
         <v>1.0</v>
       </c>
-      <c r="B50" s="67" t="s">
+      <c r="B50" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="C50" s="74"/>
-      <c r="D50" s="77">
+      <c r="C50" s="75"/>
+      <c r="D50" s="78">
         <v>1.0</v>
       </c>
-      <c r="E50" s="67" t="s">
+      <c r="E50" s="69" t="s">
         <v>119</v>
       </c>
-      <c r="F50" s="79"/>
+      <c r="F50" s="80"/>
     </row>
     <row r="51">
-      <c r="A51" s="94">
+      <c r="A51" s="95">
         <v>2.0</v>
       </c>
-      <c r="B51" s="78" t="s">
+      <c r="B51" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="C51" s="74"/>
-      <c r="D51" s="77">
+      <c r="C51" s="75"/>
+      <c r="D51" s="78">
         <v>2.0</v>
       </c>
-      <c r="E51" s="78" t="s">
+      <c r="E51" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="F51" s="79"/>
+      <c r="F51" s="80"/>
     </row>
     <row r="52">
-      <c r="A52" s="79"/>
-      <c r="B52" s="79"/>
-      <c r="C52" s="79"/>
-      <c r="D52" s="79"/>
-      <c r="E52" s="79"/>
-      <c r="F52" s="79"/>
+      <c r="A52" s="80"/>
+      <c r="B52" s="80"/>
+      <c r="C52" s="80"/>
+      <c r="D52" s="80"/>
+      <c r="E52" s="80"/>
+      <c r="F52" s="80"/>
     </row>
     <row r="53">
-      <c r="A53" s="79"/>
-      <c r="B53" s="79"/>
-      <c r="C53" s="79"/>
-      <c r="D53" s="79"/>
-      <c r="E53" s="79"/>
-      <c r="F53" s="79"/>
+      <c r="A53" s="80"/>
+      <c r="B53" s="80"/>
+      <c r="C53" s="80"/>
+      <c r="D53" s="80"/>
+      <c r="E53" s="80"/>
+      <c r="F53" s="80"/>
     </row>
     <row r="54">
-      <c r="A54" s="80"/>
-      <c r="B54" s="80"/>
-      <c r="C54" s="80"/>
-      <c r="D54" s="80"/>
-      <c r="E54" s="80"/>
-      <c r="F54" s="79"/>
+      <c r="A54" s="81"/>
+      <c r="B54" s="81"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81"/>
+      <c r="E54" s="81"/>
+      <c r="F54" s="80"/>
     </row>
     <row r="55">
-      <c r="A55" s="81" t="s">
+      <c r="A55" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="B55" s="82" t="s">
+      <c r="B55" s="83" t="s">
         <v>120</v>
       </c>
-      <c r="E55" s="83"/>
-      <c r="F55" s="79"/>
+      <c r="E55" s="84"/>
+      <c r="F55" s="80"/>
     </row>
     <row r="56">
       <c r="A56" s="39"/>
@@ -4977,42 +4962,42 @@
       <c r="E56" s="8"/>
     </row>
     <row r="57">
-      <c r="A57" s="84" t="s">
+      <c r="A57" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="B57" s="80" t="s">
+      <c r="B57" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="85"/>
-      <c r="D57" s="86" t="s">
+      <c r="C57" s="86"/>
+      <c r="D57" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="E57" s="87" t="s">
+      <c r="E57" s="88" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="80"/>
-      <c r="B58" s="80"/>
-      <c r="C58" s="80"/>
-      <c r="D58" s="80"/>
-      <c r="E58" s="80"/>
+      <c r="A58" s="81"/>
+      <c r="B58" s="81"/>
+      <c r="C58" s="81"/>
+      <c r="D58" s="81"/>
+      <c r="E58" s="81"/>
     </row>
     <row r="59">
-      <c r="A59" s="95" t="s">
+      <c r="A59" s="96" t="s">
         <v>121</v>
       </c>
-      <c r="B59" s="89" t="s">
+      <c r="B59" s="90" t="s">
         <v>53</v>
       </c>
       <c r="C59" s="8"/>
-      <c r="D59" s="90" t="s">
+      <c r="D59" s="91" t="s">
         <v>54</v>
       </c>
       <c r="E59" s="8"/>
     </row>
     <row r="60">
-      <c r="A60" s="91">
+      <c r="A60" s="92">
         <v>1.0</v>
       </c>
       <c r="B60" s="50" t="s">
@@ -5025,7 +5010,7 @@
       <c r="E60" s="5"/>
     </row>
     <row r="61">
-      <c r="A61" s="91">
+      <c r="A61" s="92">
         <v>2.0</v>
       </c>
       <c r="B61" s="50" t="s">
@@ -5038,7 +5023,7 @@
       <c r="E61" s="5"/>
     </row>
     <row r="62">
-      <c r="A62" s="91">
+      <c r="A62" s="92">
         <v>3.0</v>
       </c>
       <c r="B62" s="50" t="s">
@@ -5060,46 +5045,46 @@
       <c r="B64" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C64" s="53" t="s">
+      <c r="C64" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D64" s="72" t="s">
+      <c r="D64" s="73" t="s">
         <v>125</v>
       </c>
       <c r="E64" s="5"/>
       <c r="F64" s="14"/>
     </row>
     <row r="65">
-      <c r="A65" s="55" t="s">
+      <c r="A65" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B65" s="56" t="s">
+      <c r="B65" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C65" s="57" t="s">
+      <c r="C65" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="D65" s="58" t="s">
+      <c r="D65" s="60" t="s">
         <v>96</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="14"/>
     </row>
     <row r="66">
-      <c r="A66" s="59" t="s">
+      <c r="A66" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="60"/>
-      <c r="C66" s="61"/>
-      <c r="D66" s="62" t="s">
+      <c r="B66" s="62"/>
+      <c r="C66" s="63"/>
+      <c r="D66" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="E66" s="63" t="s">
+      <c r="E66" s="65" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="67">
-      <c r="F67" s="79"/>
+      <c r="F67" s="80"/>
     </row>
     <row r="68">
       <c r="A68" s="15" t="s">
@@ -5111,96 +5096,96 @@
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
-      <c r="F68" s="79"/>
+      <c r="F68" s="80"/>
     </row>
     <row r="69">
-      <c r="F69" s="79"/>
+      <c r="F69" s="80"/>
     </row>
     <row r="70">
-      <c r="A70" s="64" t="s">
+      <c r="A70" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="B70" s="93" t="s">
+      <c r="B70" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="C70" s="74"/>
-      <c r="D70" s="75" t="s">
+      <c r="C70" s="75"/>
+      <c r="D70" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="E70" s="76" t="s">
+      <c r="E70" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="F70" s="79"/>
+      <c r="F70" s="80"/>
     </row>
     <row r="71">
-      <c r="A71" s="94">
+      <c r="A71" s="95">
         <v>1.0</v>
       </c>
-      <c r="B71" s="78" t="s">
+      <c r="B71" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="C71" s="74"/>
-      <c r="D71" s="77">
+      <c r="C71" s="75"/>
+      <c r="D71" s="78">
         <v>1.0</v>
       </c>
-      <c r="E71" s="67" t="s">
+      <c r="E71" s="69" t="s">
         <v>127</v>
       </c>
-      <c r="F71" s="79"/>
+      <c r="F71" s="80"/>
     </row>
     <row r="72">
-      <c r="A72" s="94">
+      <c r="A72" s="95">
         <v>2.0</v>
       </c>
-      <c r="B72" s="78" t="s">
+      <c r="B72" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="C72" s="74"/>
-      <c r="D72" s="77">
+      <c r="C72" s="75"/>
+      <c r="D72" s="78">
         <v>2.0</v>
       </c>
-      <c r="E72" s="67" t="s">
+      <c r="E72" s="69" t="s">
         <v>128</v>
       </c>
-      <c r="F72" s="79"/>
+      <c r="F72" s="80"/>
     </row>
     <row r="73">
-      <c r="A73" s="94">
+      <c r="A73" s="95">
         <v>3.0</v>
       </c>
-      <c r="B73" s="78" t="s">
+      <c r="B73" s="79" t="s">
         <v>129</v>
       </c>
-      <c r="C73" s="79"/>
-      <c r="D73" s="79"/>
-      <c r="E73" s="79"/>
-      <c r="F73" s="79"/>
+      <c r="C73" s="80"/>
+      <c r="D73" s="80"/>
+      <c r="E73" s="80"/>
+      <c r="F73" s="80"/>
     </row>
     <row r="74">
-      <c r="A74" s="79"/>
-      <c r="B74" s="79"/>
-      <c r="C74" s="79"/>
-      <c r="D74" s="79"/>
-      <c r="E74" s="79"/>
-      <c r="F74" s="79"/>
+      <c r="A74" s="80"/>
+      <c r="B74" s="80"/>
+      <c r="C74" s="80"/>
+      <c r="D74" s="80"/>
+      <c r="E74" s="80"/>
+      <c r="F74" s="80"/>
     </row>
     <row r="75">
-      <c r="A75" s="80"/>
-      <c r="B75" s="80"/>
-      <c r="C75" s="80"/>
-      <c r="D75" s="80"/>
-      <c r="E75" s="80"/>
-      <c r="F75" s="79"/>
+      <c r="A75" s="81"/>
+      <c r="B75" s="81"/>
+      <c r="C75" s="81"/>
+      <c r="D75" s="81"/>
+      <c r="E75" s="81"/>
+      <c r="F75" s="80"/>
     </row>
     <row r="76">
-      <c r="A76" s="81" t="s">
+      <c r="A76" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="B76" s="82" t="s">
+      <c r="B76" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="E76" s="83"/>
-      <c r="F76" s="79"/>
+      <c r="E76" s="84"/>
+      <c r="F76" s="80"/>
     </row>
     <row r="77">
       <c r="A77" s="39"/>
@@ -5208,48 +5193,48 @@
       <c r="C77" s="41"/>
       <c r="D77" s="41"/>
       <c r="E77" s="8"/>
-      <c r="F77" s="79"/>
+      <c r="F77" s="80"/>
     </row>
     <row r="78">
-      <c r="A78" s="84" t="s">
+      <c r="A78" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="B78" s="80" t="s">
+      <c r="B78" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="C78" s="85"/>
-      <c r="D78" s="86" t="s">
+      <c r="C78" s="86"/>
+      <c r="D78" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="E78" s="87" t="s">
+      <c r="E78" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="F78" s="79"/>
+      <c r="F78" s="80"/>
     </row>
     <row r="79">
-      <c r="A79" s="80"/>
-      <c r="B79" s="80"/>
-      <c r="C79" s="80"/>
-      <c r="D79" s="80"/>
-      <c r="E79" s="80"/>
-      <c r="F79" s="79"/>
+      <c r="A79" s="81"/>
+      <c r="B79" s="81"/>
+      <c r="C79" s="81"/>
+      <c r="D79" s="81"/>
+      <c r="E79" s="81"/>
+      <c r="F79" s="80"/>
     </row>
     <row r="80">
-      <c r="A80" s="95" t="s">
+      <c r="A80" s="96" t="s">
         <v>121</v>
       </c>
-      <c r="B80" s="89" t="s">
+      <c r="B80" s="90" t="s">
         <v>53</v>
       </c>
       <c r="C80" s="8"/>
-      <c r="D80" s="90" t="s">
+      <c r="D80" s="91" t="s">
         <v>54</v>
       </c>
       <c r="E80" s="8"/>
-      <c r="F80" s="79"/>
+      <c r="F80" s="80"/>
     </row>
     <row r="81">
-      <c r="A81" s="91">
+      <c r="A81" s="92">
         <v>1.0</v>
       </c>
       <c r="B81" s="50" t="s">
@@ -5260,10 +5245,10 @@
         <v>56</v>
       </c>
       <c r="E81" s="5"/>
-      <c r="F81" s="79"/>
+      <c r="F81" s="80"/>
     </row>
     <row r="82">
-      <c r="A82" s="91">
+      <c r="A82" s="92">
         <v>2.0</v>
       </c>
       <c r="B82" s="50" t="s">
@@ -5274,10 +5259,10 @@
         <v>114</v>
       </c>
       <c r="E82" s="5"/>
-      <c r="F82" s="79"/>
+      <c r="F82" s="80"/>
     </row>
     <row r="83">
-      <c r="A83" s="91">
+      <c r="A83" s="92">
         <v>3.0</v>
       </c>
       <c r="B83" s="50" t="s">
@@ -5288,7 +5273,7 @@
         <v>131</v>
       </c>
       <c r="E83" s="5"/>
-      <c r="F83" s="79"/>
+      <c r="F83" s="80"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
@@ -5297,39 +5282,39 @@
       <c r="B85" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C85" s="53" t="s">
+      <c r="C85" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D85" s="72" t="s">
+      <c r="D85" s="73" t="s">
         <v>133</v>
       </c>
       <c r="E85" s="5"/>
     </row>
     <row r="86">
-      <c r="A86" s="55" t="s">
+      <c r="A86" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B86" s="56" t="s">
+      <c r="B86" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C86" s="57" t="s">
+      <c r="C86" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="D86" s="58" t="s">
+      <c r="D86" s="60" t="s">
         <v>96</v>
       </c>
       <c r="E86" s="8"/>
     </row>
     <row r="87">
-      <c r="A87" s="59" t="s">
+      <c r="A87" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="B87" s="60"/>
-      <c r="C87" s="61"/>
-      <c r="D87" s="62" t="s">
+      <c r="B87" s="62"/>
+      <c r="C87" s="63"/>
+      <c r="D87" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="E87" s="63" t="s">
+      <c r="E87" s="65" t="s">
         <v>10</v>
       </c>
     </row>
@@ -5345,79 +5330,79 @@
       <c r="E89" s="14"/>
     </row>
     <row r="91">
-      <c r="A91" s="64" t="s">
+      <c r="A91" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="B91" s="65" t="s">
+      <c r="B91" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C91" s="74"/>
-      <c r="D91" s="75" t="s">
+      <c r="C91" s="75"/>
+      <c r="D91" s="76" t="s">
         <v>134</v>
       </c>
-      <c r="E91" s="76" t="s">
+      <c r="E91" s="77" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="66">
+      <c r="A92" s="68">
         <v>1.0</v>
       </c>
-      <c r="B92" s="67" t="s">
+      <c r="B92" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="C92" s="74"/>
-      <c r="D92" s="77">
+      <c r="C92" s="75"/>
+      <c r="D92" s="78">
         <v>1.0</v>
       </c>
-      <c r="E92" s="67" t="s">
+      <c r="E92" s="69" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="68">
+      <c r="A93" s="70">
         <v>2.0</v>
       </c>
-      <c r="B93" s="69" t="s">
+      <c r="B93" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="C93" s="74"/>
-      <c r="D93" s="77">
+      <c r="C93" s="75"/>
+      <c r="D93" s="78">
         <v>2.0</v>
       </c>
-      <c r="E93" s="67" t="s">
+      <c r="E93" s="69" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="79"/>
-      <c r="B94" s="79"/>
-      <c r="C94" s="79"/>
-      <c r="D94" s="79"/>
-      <c r="E94" s="79"/>
+      <c r="A94" s="80"/>
+      <c r="B94" s="80"/>
+      <c r="C94" s="80"/>
+      <c r="D94" s="80"/>
+      <c r="E94" s="80"/>
     </row>
     <row r="95">
-      <c r="A95" s="79"/>
-      <c r="B95" s="79"/>
-      <c r="C95" s="79"/>
-      <c r="D95" s="79"/>
-      <c r="E95" s="79"/>
+      <c r="A95" s="80"/>
+      <c r="B95" s="80"/>
+      <c r="C95" s="80"/>
+      <c r="D95" s="80"/>
+      <c r="E95" s="80"/>
     </row>
     <row r="96">
-      <c r="A96" s="80"/>
-      <c r="B96" s="80"/>
-      <c r="C96" s="80"/>
-      <c r="D96" s="80"/>
-      <c r="E96" s="80"/>
+      <c r="A96" s="81"/>
+      <c r="B96" s="81"/>
+      <c r="C96" s="81"/>
+      <c r="D96" s="81"/>
+      <c r="E96" s="81"/>
     </row>
     <row r="97">
-      <c r="A97" s="81" t="s">
+      <c r="A97" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="B97" s="82" t="s">
+      <c r="B97" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="E97" s="83"/>
+      <c r="E97" s="84"/>
     </row>
     <row r="98">
       <c r="A98" s="39"/>
@@ -5427,42 +5412,42 @@
       <c r="E98" s="8"/>
     </row>
     <row r="99">
-      <c r="A99" s="84" t="s">
+      <c r="A99" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="B99" s="80" t="s">
+      <c r="B99" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="C99" s="85"/>
-      <c r="D99" s="86" t="s">
+      <c r="C99" s="86"/>
+      <c r="D99" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="E99" s="87" t="s">
+      <c r="E99" s="88" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="80"/>
-      <c r="B100" s="80"/>
-      <c r="C100" s="80"/>
-      <c r="D100" s="80"/>
-      <c r="E100" s="80"/>
+      <c r="A100" s="81"/>
+      <c r="B100" s="81"/>
+      <c r="C100" s="81"/>
+      <c r="D100" s="81"/>
+      <c r="E100" s="81"/>
     </row>
     <row r="101">
-      <c r="A101" s="88" t="s">
+      <c r="A101" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="B101" s="89" t="s">
+      <c r="B101" s="90" t="s">
         <v>53</v>
       </c>
       <c r="C101" s="8"/>
-      <c r="D101" s="90" t="s">
+      <c r="D101" s="91" t="s">
         <v>54</v>
       </c>
       <c r="E101" s="8"/>
     </row>
     <row r="102">
-      <c r="A102" s="91">
+      <c r="A102" s="92">
         <v>1.0</v>
       </c>
       <c r="B102" s="50" t="s">
@@ -5475,7 +5460,7 @@
       <c r="E102" s="5"/>
     </row>
     <row r="103">
-      <c r="A103" s="91">
+      <c r="A103" s="92">
         <v>2.0</v>
       </c>
       <c r="B103" s="50" t="s">
@@ -5488,7 +5473,7 @@
       <c r="E103" s="5"/>
     </row>
     <row r="104">
-      <c r="A104" s="91">
+      <c r="A104" s="92">
         <v>3.0</v>
       </c>
       <c r="B104" s="50" t="s">
@@ -5507,39 +5492,39 @@
       <c r="B107" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C107" s="53" t="s">
+      <c r="C107" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D107" s="72" t="s">
+      <c r="D107" s="73" t="s">
         <v>139</v>
       </c>
       <c r="E107" s="5"/>
     </row>
     <row r="108">
-      <c r="A108" s="55" t="s">
+      <c r="A108" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B108" s="56" t="s">
+      <c r="B108" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C108" s="57" t="s">
+      <c r="C108" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="D108" s="58" t="s">
+      <c r="D108" s="60" t="s">
         <v>96</v>
       </c>
       <c r="E108" s="8"/>
     </row>
     <row r="109">
-      <c r="A109" s="59" t="s">
+      <c r="A109" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="B109" s="60"/>
-      <c r="C109" s="61"/>
-      <c r="D109" s="62" t="s">
+      <c r="B109" s="62"/>
+      <c r="C109" s="63"/>
+      <c r="D109" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="E109" s="63" t="s">
+      <c r="E109" s="65" t="s">
         <v>10</v>
       </c>
     </row>
@@ -5555,83 +5540,83 @@
       <c r="E111" s="14"/>
     </row>
     <row r="113">
-      <c r="A113" s="64" t="s">
+      <c r="A113" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="B113" s="93" t="s">
+      <c r="B113" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="C113" s="74"/>
-      <c r="D113" s="75" t="s">
+      <c r="C113" s="75"/>
+      <c r="D113" s="76" t="s">
         <v>140</v>
       </c>
-      <c r="E113" s="76" t="s">
+      <c r="E113" s="77" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="94">
+      <c r="A114" s="95">
         <v>1.0</v>
       </c>
-      <c r="B114" s="78" t="s">
+      <c r="B114" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="C114" s="74"/>
-      <c r="D114" s="77">
+      <c r="C114" s="75"/>
+      <c r="D114" s="78">
         <v>1.0</v>
       </c>
-      <c r="E114" s="67" t="s">
+      <c r="E114" s="69" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="94">
+      <c r="A115" s="95">
         <v>2.0</v>
       </c>
-      <c r="B115" s="78" t="s">
+      <c r="B115" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="C115" s="74"/>
-      <c r="D115" s="77">
+      <c r="C115" s="75"/>
+      <c r="D115" s="78">
         <v>2.0</v>
       </c>
-      <c r="E115" s="67" t="s">
+      <c r="E115" s="69" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="94">
+      <c r="A116" s="95">
         <v>3.0</v>
       </c>
-      <c r="B116" s="78" t="s">
+      <c r="B116" s="79" t="s">
         <v>129</v>
       </c>
-      <c r="C116" s="79"/>
-      <c r="D116" s="79"/>
-      <c r="E116" s="79"/>
+      <c r="C116" s="80"/>
+      <c r="D116" s="80"/>
+      <c r="E116" s="80"/>
     </row>
     <row r="117">
-      <c r="A117" s="79"/>
-      <c r="B117" s="79"/>
-      <c r="C117" s="79"/>
-      <c r="D117" s="79"/>
-      <c r="E117" s="79"/>
+      <c r="A117" s="80"/>
+      <c r="B117" s="80"/>
+      <c r="C117" s="80"/>
+      <c r="D117" s="80"/>
+      <c r="E117" s="80"/>
     </row>
     <row r="118">
-      <c r="A118" s="80"/>
-      <c r="B118" s="80"/>
-      <c r="C118" s="80"/>
-      <c r="D118" s="80"/>
-      <c r="E118" s="80"/>
+      <c r="A118" s="81"/>
+      <c r="B118" s="81"/>
+      <c r="C118" s="81"/>
+      <c r="D118" s="81"/>
+      <c r="E118" s="81"/>
     </row>
     <row r="119">
-      <c r="A119" s="81" t="s">
+      <c r="A119" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="B119" s="82" t="s">
+      <c r="B119" s="83" t="s">
         <v>130</v>
       </c>
-      <c r="E119" s="83"/>
+      <c r="E119" s="84"/>
     </row>
     <row r="120">
       <c r="A120" s="39"/>
@@ -5641,42 +5626,42 @@
       <c r="E120" s="8"/>
     </row>
     <row r="121">
-      <c r="A121" s="84" t="s">
+      <c r="A121" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="B121" s="80" t="s">
+      <c r="B121" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="C121" s="85"/>
-      <c r="D121" s="86" t="s">
+      <c r="C121" s="86"/>
+      <c r="D121" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="E121" s="87" t="s">
+      <c r="E121" s="88" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="80"/>
-      <c r="B122" s="80"/>
-      <c r="C122" s="80"/>
-      <c r="D122" s="80"/>
-      <c r="E122" s="80"/>
+      <c r="A122" s="81"/>
+      <c r="B122" s="81"/>
+      <c r="C122" s="81"/>
+      <c r="D122" s="81"/>
+      <c r="E122" s="81"/>
     </row>
     <row r="123">
-      <c r="A123" s="95" t="s">
+      <c r="A123" s="96" t="s">
         <v>121</v>
       </c>
-      <c r="B123" s="89" t="s">
+      <c r="B123" s="90" t="s">
         <v>53</v>
       </c>
       <c r="C123" s="8"/>
-      <c r="D123" s="90" t="s">
+      <c r="D123" s="91" t="s">
         <v>54</v>
       </c>
       <c r="E123" s="8"/>
     </row>
     <row r="124">
-      <c r="A124" s="91">
+      <c r="A124" s="92">
         <v>1.0</v>
       </c>
       <c r="B124" s="50" t="s">
@@ -5689,7 +5674,7 @@
       <c r="E124" s="5"/>
     </row>
     <row r="125">
-      <c r="A125" s="91">
+      <c r="A125" s="92">
         <v>2.0</v>
       </c>
       <c r="B125" s="50" t="s">
@@ -5702,7 +5687,7 @@
       <c r="E125" s="5"/>
     </row>
     <row r="126">
-      <c r="A126" s="96">
+      <c r="A126" s="97">
         <v>3.0</v>
       </c>
       <c r="B126" s="50" t="s">
@@ -5715,7 +5700,7 @@
       <c r="E126" s="5"/>
     </row>
     <row r="127">
-      <c r="A127" s="97">
+      <c r="A127" s="98">
         <v>4.0</v>
       </c>
       <c r="B127" s="50" t="s">
@@ -5728,7 +5713,7 @@
       <c r="E127" s="5"/>
     </row>
     <row r="128">
-      <c r="A128" s="97">
+      <c r="A128" s="98">
         <v>5.0</v>
       </c>
       <c r="B128" s="50" t="s">
@@ -5741,20 +5726,20 @@
       <c r="E128" s="5"/>
     </row>
     <row r="129">
-      <c r="A129" s="97">
+      <c r="A129" s="98">
         <v>6.0</v>
       </c>
-      <c r="B129" s="98" t="s">
+      <c r="B129" s="99" t="s">
         <v>122</v>
       </c>
       <c r="C129" s="37"/>
-      <c r="D129" s="98" t="s">
+      <c r="D129" s="99" t="s">
         <v>114</v>
       </c>
       <c r="E129" s="37"/>
     </row>
     <row r="130">
-      <c r="A130" s="97">
+      <c r="A130" s="98">
         <v>7.0</v>
       </c>
       <c r="B130" s="50" t="s">
@@ -5817,54 +5802,44 @@
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="M29:N29"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B39:C39"/>
     <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D39:E39"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="D60:E60"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="D104:E104"/>
     <mergeCell ref="D107:E107"/>
     <mergeCell ref="D108:E108"/>
     <mergeCell ref="A119:A120"/>
     <mergeCell ref="B119:E120"/>
     <mergeCell ref="B123:C123"/>
     <mergeCell ref="D123:E123"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D124:E124"/>
     <mergeCell ref="B124:C124"/>
-    <mergeCell ref="D124:E124"/>
     <mergeCell ref="B125:C125"/>
     <mergeCell ref="D125:E125"/>
+    <mergeCell ref="B126:C126"/>
     <mergeCell ref="D126:E126"/>
+    <mergeCell ref="B127:C127"/>
     <mergeCell ref="D127:E127"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="B34:E35"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="B55:E56"/>
     <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="A76:A77"/>
     <mergeCell ref="B61:C61"/>
     <mergeCell ref="D61:E61"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="A76:A77"/>
     <mergeCell ref="B76:E77"/>
     <mergeCell ref="B80:C80"/>
     <mergeCell ref="D80:E80"/>
@@ -5872,16 +5847,26 @@
     <mergeCell ref="D81:E81"/>
     <mergeCell ref="B82:C82"/>
     <mergeCell ref="D82:E82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:E83"/>
     <mergeCell ref="D85:E85"/>
     <mergeCell ref="D86:E86"/>
     <mergeCell ref="A97:A98"/>
     <mergeCell ref="B97:E98"/>
     <mergeCell ref="D101:E101"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:E83"/>
     <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="D130:E130"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -6005,10 +5990,10 @@
       <c r="B7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="99" t="s">
+      <c r="D7" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="100" t="s">
+      <c r="E7" s="101" t="s">
         <v>18</v>
       </c>
     </row>
@@ -6019,18 +6004,18 @@
       <c r="B8" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D8" s="101">
+      <c r="D8" s="102">
         <v>1.0</v>
       </c>
-      <c r="E8" s="102" t="s">
+      <c r="E8" s="103" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
-      <c r="D9" s="101">
+      <c r="D9" s="102">
         <v>2.0</v>
       </c>
-      <c r="E9" s="102" t="s">
+      <c r="E9" s="103" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6407,10 +6392,10 @@
       <c r="B28" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D28" s="103">
+      <c r="D28" s="104">
         <v>1.0</v>
       </c>
-      <c r="E28" s="104" t="s">
+      <c r="E28" s="105" t="s">
         <v>157</v>
       </c>
       <c r="G28" s="38"/>
@@ -6571,7 +6556,7 @@
       <c r="B43" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C43" s="105" t="s">
+      <c r="C43" s="106" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="7" t="s">
@@ -6626,10 +6611,10 @@
       <c r="B49" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D49" s="103">
+      <c r="D49" s="104">
         <v>1.0</v>
       </c>
-      <c r="E49" s="104" t="s">
+      <c r="E49" s="105" t="s">
         <v>160</v>
       </c>
     </row>
@@ -6752,7 +6737,7 @@
       <c r="B63" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C63" s="105" t="s">
+      <c r="C63" s="106" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="7" t="s">
@@ -6807,10 +6792,10 @@
       <c r="B69" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D69" s="103">
+      <c r="D69" s="104">
         <v>1.0</v>
       </c>
-      <c r="E69" s="104" t="s">
+      <c r="E69" s="105" t="s">
         <v>160</v>
       </c>
     </row>
@@ -6823,8 +6808,8 @@
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
-      <c r="D71" s="106"/>
-      <c r="E71" s="106"/>
+      <c r="D71" s="107"/>
+      <c r="E71" s="107"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="34" t="s">
@@ -6900,14 +6885,14 @@
       <c r="E78" s="5"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" s="107">
+      <c r="A79" s="108">
         <v>3.0</v>
       </c>
-      <c r="B79" s="98" t="s">
+      <c r="B79" s="99" t="s">
         <v>153</v>
       </c>
       <c r="C79" s="37"/>
-      <c r="D79" s="98" t="s">
+      <c r="D79" s="99" t="s">
         <v>168</v>
       </c>
       <c r="E79" s="37"/>
@@ -8054,7 +8039,7 @@
     </row>
     <row r="6" ht="14.25" customHeight="1"/>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="108" t="s">
+      <c r="A7" s="109" t="s">
         <v>173</v>
       </c>
       <c r="B7" s="12" t="s">
@@ -8078,7 +8063,7 @@
       <c r="E8" s="19"/>
     </row>
     <row r="9" ht="21.0" customHeight="1">
-      <c r="A9" s="109">
+      <c r="A9" s="110">
         <v>2.0</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -8323,7 +8308,7 @@
       <c r="C21" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="110" t="s">
+      <c r="D21" s="111" t="s">
         <v>5</v>
       </c>
       <c r="G21" s="31"/>
@@ -8438,7 +8423,7 @@
       <c r="N27" s="5"/>
     </row>
     <row r="28" ht="25.5" customHeight="1">
-      <c r="A28" s="109">
+      <c r="A28" s="110">
         <v>2.0</v>
       </c>
       <c r="B28" s="19" t="s">
@@ -8508,7 +8493,7 @@
     </row>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="111" t="s">
+      <c r="A35" s="112" t="s">
         <v>186</v>
       </c>
       <c r="B35" s="47" t="s">
@@ -9623,7 +9608,7 @@
       <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="110" t="s">
+      <c r="D2" s="111" t="s">
         <v>95</v>
       </c>
     </row>
@@ -9703,15 +9688,15 @@
       <c r="B8" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="D8" s="112" t="s">
+      <c r="D8" s="113" t="s">
         <v>192</v>
       </c>
-      <c r="E8" s="112" t="s">
+      <c r="E8" s="113" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="1">
-      <c r="A9" s="109">
+      <c r="A9" s="110">
         <v>2.0</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -9719,7 +9704,7 @@
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="109">
+      <c r="A10" s="110">
         <v>3.0</v>
       </c>
       <c r="B10" s="19" t="s">
@@ -9727,7 +9712,7 @@
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="109">
+      <c r="A11" s="110">
         <v>4.0</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -9736,7 +9721,7 @@
       <c r="F11" s="13"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="C12" s="70"/>
+      <c r="C12" s="72"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="F13" s="13"/>
@@ -9990,7 +9975,7 @@
       <c r="C23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="110" t="s">
+      <c r="D23" s="111" t="s">
         <v>95</v>
       </c>
       <c r="G23" s="31"/>
@@ -10093,10 +10078,10 @@
       <c r="B29" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="D29" s="112" t="s">
+      <c r="D29" s="113" t="s">
         <v>192</v>
       </c>
-      <c r="E29" s="112" t="s">
+      <c r="E29" s="113" t="s">
         <v>192</v>
       </c>
       <c r="G29" s="38"/>
@@ -10109,7 +10094,7 @@
       <c r="N29" s="5"/>
     </row>
     <row r="30" ht="25.5" customHeight="1">
-      <c r="A30" s="109">
+      <c r="A30" s="110">
         <v>2.0</v>
       </c>
       <c r="B30" s="19" t="s">
@@ -10125,7 +10110,7 @@
       <c r="N30" s="5"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="109">
+      <c r="A31" s="110">
         <v>3.0</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -10133,7 +10118,7 @@
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="109">
+      <c r="A32" s="110">
         <v>4.0</v>
       </c>
       <c r="B32" s="19" t="s">
@@ -10227,7 +10212,7 @@
       <c r="C42" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="110" t="s">
+      <c r="D42" s="111" t="s">
         <v>95</v>
       </c>
     </row>
@@ -10278,15 +10263,15 @@
       <c r="B48" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="D48" s="112" t="s">
+      <c r="D48" s="113" t="s">
         <v>192</v>
       </c>
-      <c r="E48" s="112" t="s">
+      <c r="E48" s="113" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="109">
+      <c r="A49" s="110">
         <v>2.0</v>
       </c>
       <c r="B49" s="19" t="s">
@@ -10294,7 +10279,7 @@
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="109">
+      <c r="A50" s="110">
         <v>3.0</v>
       </c>
       <c r="B50" s="19" t="s">
@@ -10302,7 +10287,7 @@
       </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="109">
+      <c r="A51" s="110">
         <v>4.0</v>
       </c>
       <c r="B51" s="19" t="s">
@@ -10348,11 +10333,11 @@
       <c r="A57" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="B57" s="113" t="s">
+      <c r="B57" s="114" t="s">
         <v>53</v>
       </c>
       <c r="C57" s="5"/>
-      <c r="D57" s="114" t="s">
+      <c r="D57" s="115" t="s">
         <v>54</v>
       </c>
       <c r="E57" s="5"/>

</xml_diff>